<commit_message>
Added rows (placeholders) for min/max chem computations
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" activeTab="4"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="79">
   <si>
     <t>ER</t>
   </si>
@@ -250,7 +250,16 @@
     <t>nominal</t>
   </si>
   <si>
-    <t>max (min?)</t>
+    <t>min_MHR</t>
+  </si>
+  <si>
+    <t>max_MHR</t>
+  </si>
+  <si>
+    <t>min_IHR</t>
+  </si>
+  <si>
+    <t>max_IHR</t>
   </si>
 </sst>
 </file>
@@ -548,6 +557,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -568,9 +580,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -1970,20 +1979,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4"/>
@@ -2012,7 +2021,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>0.25</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2034,7 +2043,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2054,7 +2063,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2074,7 +2083,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2094,7 +2103,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2114,7 +2123,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2134,7 +2143,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2154,7 +2163,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2174,7 +2183,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2194,7 +2203,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2214,7 +2223,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2234,7 +2243,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2254,7 +2263,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2274,7 +2283,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2294,7 +2303,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2374,31 +2383,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2424,7 +2433,7 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="25">
+      <c r="A3" s="26">
         <v>0.3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2457,7 +2466,7 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -2478,7 +2487,7 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -2499,7 +2508,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2520,7 +2529,7 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -2541,7 +2550,7 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -2562,7 +2571,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -2583,7 +2592,7 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -2604,7 +2613,7 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2625,7 +2634,7 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2646,7 +2655,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -2667,7 +2676,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2688,7 +2697,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -2709,7 +2718,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2730,7 +2739,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -3591,31 +3600,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3643,7 +3652,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3668,7 +3677,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -3691,7 +3700,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3714,7 +3723,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -3737,7 +3746,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3760,7 +3769,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -3783,7 +3792,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -3806,7 +3815,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -3827,7 +3836,7 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -3850,7 +3859,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -3873,7 +3882,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -3896,7 +3905,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -3919,7 +3928,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3942,7 +3951,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3965,7 +3974,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4074,31 +4083,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4126,7 +4135,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4151,7 +4160,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4174,7 +4183,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4197,7 +4206,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -4220,7 +4229,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -4243,7 +4252,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4266,7 +4275,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4289,7 +4298,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4312,7 +4321,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -4335,7 +4344,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -4358,7 +4367,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4381,7 +4390,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -4404,7 +4413,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4427,7 +4436,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4450,7 +4459,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4494,10 +4503,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4510,14 +4519,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="26"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -4961,11 +4970,22 @@
       <c r="A28" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="27">
-        <v>187095000000</v>
-      </c>
-      <c r="E28" s="27">
-        <v>138642.1</v>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added FPVA 1iter min/max FFR30 results to table
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" activeTab="4"/>
+    <workbookView xWindow="40" yWindow="1660" windowWidth="25360" windowHeight="15820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ER25" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="82">
   <si>
     <t>ER</t>
   </si>
@@ -260,6 +260,15 @@
   </si>
   <si>
     <t>max_IHR</t>
+  </si>
+  <si>
+    <t>full</t>
+  </si>
+  <si>
+    <t>P(exit)</t>
+  </si>
+  <si>
+    <t>SupersonicVolume</t>
   </si>
 </sst>
 </file>
@@ -518,7 +527,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -556,9 +565,6 @@
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1979,20 +1985,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4"/>
@@ -2021,7 +2027,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>0.25</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2043,7 +2049,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2063,7 +2069,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2083,7 +2089,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2103,7 +2109,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2123,7 +2129,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2143,7 +2149,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2163,7 +2169,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2183,7 +2189,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2203,7 +2209,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2223,7 +2229,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2243,7 +2249,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2263,7 +2269,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2283,7 +2289,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2303,7 +2309,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2383,31 +2389,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2433,7 +2439,7 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="26">
+      <c r="A3" s="25">
         <v>0.3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2466,7 +2472,7 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -2487,7 +2493,7 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -2508,7 +2514,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2529,7 +2535,7 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -2550,7 +2556,7 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -2571,7 +2577,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -2592,7 +2598,7 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -2613,7 +2619,7 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2634,7 +2640,7 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2655,7 +2661,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -2676,7 +2682,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2697,7 +2703,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -2718,7 +2724,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2739,7 +2745,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -3600,31 +3606,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3652,7 +3658,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3677,7 +3683,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -3700,7 +3706,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3723,7 +3729,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -3746,7 +3752,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3769,7 +3775,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -3792,7 +3798,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -3815,7 +3821,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -3836,7 +3842,7 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -3859,7 +3865,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -3882,7 +3888,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -3905,7 +3911,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -3928,7 +3934,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3951,7 +3957,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3974,7 +3980,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4083,31 +4089,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="21"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4135,7 +4141,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="22">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4160,7 +4166,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4183,7 +4189,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4206,7 +4212,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -4229,7 +4235,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -4252,7 +4258,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4275,7 +4281,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="23"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4298,7 +4304,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="23"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4321,7 +4327,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="23"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -4344,7 +4350,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="23"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -4367,7 +4373,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="23"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4390,7 +4396,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="23"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -4413,7 +4419,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="23"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4436,7 +4442,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="23"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4459,7 +4465,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="23"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4503,10 +4509,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4518,17 +4524,21 @@
     <col min="5" max="5" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="27" t="s">
+    <row r="1" spans="1:7">
+      <c r="B1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="26"/>
+      <c r="D1" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="27"/>
-    </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" ht="32">
+      <c r="E1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
@@ -4544,8 +4554,14 @@
       <c r="E2" s="16" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="18" t="s">
         <v>74</v>
       </c>
@@ -4558,7 +4574,7 @@
         <v>162689.60000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4575,7 +4591,7 @@
         <v>182264.5</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4592,7 +4608,7 @@
         <v>196857</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4609,7 +4625,7 @@
         <v>199086</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4626,7 +4642,7 @@
         <v>193967.2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4643,7 +4659,7 @@
         <v>185925.4</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4660,7 +4676,7 @@
         <v>179938.2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4677,7 +4693,7 @@
         <v>192477.4</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4694,7 +4710,7 @@
         <v>186667.4</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4711,7 +4727,7 @@
         <v>203428.3</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4728,7 +4744,7 @@
         <v>186549.8</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4745,7 +4761,7 @@
         <v>174946.6</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4762,7 +4778,7 @@
         <v>196397.9</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>13</v>
       </c>
@@ -4970,28 +4986,51 @@
       <c r="A28" t="s">
         <v>75</v>
       </c>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
+      <c r="D28" s="14">
+        <v>184369000000</v>
+      </c>
+      <c r="E28" s="14">
+        <v>133147.79999999999</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>76</v>
       </c>
+      <c r="D29" s="14">
+        <v>290364000000</v>
+      </c>
+      <c r="E29" s="14">
+        <v>204300.5</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>77</v>
       </c>
+      <c r="D30" s="14">
+        <v>186003000000</v>
+      </c>
+      <c r="E30" s="14">
+        <v>135118.20000000001</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>78</v>
       </c>
+      <c r="D31" s="14">
+        <v>287873000000</v>
+      </c>
+      <c r="E31" s="14">
+        <v>203706.5</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Added FPVA samples exit pressure and supersonic volume results to table (no min/max yet)
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="1660" windowWidth="25360" windowHeight="15820" activeTab="4"/>
+    <workbookView xWindow="1460" yWindow="1320" windowWidth="25360" windowHeight="15820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ER25" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="83">
   <si>
     <t>ER</t>
   </si>
@@ -269,16 +269,20 @@
   </si>
   <si>
     <t>SupersonicVolume</t>
+  </si>
+  <si>
+    <t>more…</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000E+00"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -527,7 +531,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -586,6 +590,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="59">
@@ -4509,10 +4516,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4524,7 +4531,7 @@
     <col min="5" max="5" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="B1" s="26" t="s">
         <v>73</v>
       </c>
@@ -4538,7 +4545,7 @@
       </c>
       <c r="G1" s="26"/>
     </row>
-    <row r="2" spans="1:7" s="13" customFormat="1" ht="32">
+    <row r="2" spans="1:8" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
@@ -4561,7 +4568,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="A3" s="18" t="s">
         <v>74</v>
       </c>
@@ -4573,8 +4580,14 @@
       <c r="E3" s="19">
         <v>162689.60000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3">
+        <v>2.3790249999999999</v>
+      </c>
+      <c r="G3" s="27">
+        <v>98.873630000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4590,8 +4603,14 @@
       <c r="E4" s="14">
         <v>182264.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="F4">
+        <v>2.3896679999999999</v>
+      </c>
+      <c r="G4" s="27">
+        <v>98.844089999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4607,8 +4626,14 @@
       <c r="E5" s="14">
         <v>196857</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="F5">
+        <v>2.393329</v>
+      </c>
+      <c r="G5" s="27">
+        <v>98.823070000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4624,8 +4649,14 @@
       <c r="E6" s="14">
         <v>199086</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="F6">
+        <v>2.4024160000000001</v>
+      </c>
+      <c r="G6" s="27">
+        <v>98.806430000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4641,8 +4672,14 @@
       <c r="E7" s="14">
         <v>193967.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="F7">
+        <v>2.3998360000000001</v>
+      </c>
+      <c r="G7" s="27">
+        <v>98.801029999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4658,8 +4695,14 @@
       <c r="E8" s="14">
         <v>185925.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="F8">
+        <v>2.3862930000000002</v>
+      </c>
+      <c r="G8" s="27">
+        <v>98.849680000000006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4675,8 +4718,14 @@
       <c r="E9" s="14">
         <v>179938.2</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="F9">
+        <v>2.3887040000000002</v>
+      </c>
+      <c r="G9" s="27">
+        <v>98.832049999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4692,8 +4741,14 @@
       <c r="E10" s="14">
         <v>192477.4</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="F10">
+        <v>2.3894449999999998</v>
+      </c>
+      <c r="G10" s="27">
+        <v>98.840479999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4709,8 +4764,14 @@
       <c r="E11" s="14">
         <v>186667.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="F11">
+        <v>2.385821</v>
+      </c>
+      <c r="G11" s="27">
+        <v>98.856620000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4726,8 +4787,14 @@
       <c r="E12" s="14">
         <v>203428.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="F12">
+        <v>2.4035739999999999</v>
+      </c>
+      <c r="G12" s="27">
+        <v>98.772540000000006</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4743,8 +4810,14 @@
       <c r="E13" s="14">
         <v>186549.8</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="F13">
+        <v>2.3931450000000001</v>
+      </c>
+      <c r="G13" s="27">
+        <v>98.813389999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4760,8 +4833,14 @@
       <c r="E14" s="14">
         <v>174946.6</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="F14">
+        <v>2.3806240000000001</v>
+      </c>
+      <c r="G14" s="27">
+        <v>98.862359999999995</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4777,8 +4856,14 @@
       <c r="E15" s="14">
         <v>196397.9</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="F15">
+        <v>2.4004530000000002</v>
+      </c>
+      <c r="G15" s="27">
+        <v>98.794079999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
       <c r="A16">
         <v>13</v>
       </c>
@@ -4794,8 +4879,17 @@
       <c r="E16" s="14">
         <v>188740.6</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16">
+        <v>2.3944990000000002</v>
+      </c>
+      <c r="G16" s="27">
+        <v>98.821259999999995</v>
+      </c>
+      <c r="H16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>14</v>
       </c>
@@ -4811,8 +4905,14 @@
       <c r="E17" s="14">
         <v>180921.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17">
+        <v>2.388582</v>
+      </c>
+      <c r="G17" s="27">
+        <v>98.828029999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>15</v>
       </c>
@@ -4828,8 +4928,14 @@
       <c r="E18" s="14">
         <v>210981.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18">
+        <v>2.4085960000000002</v>
+      </c>
+      <c r="G18" s="27">
+        <v>98.773750000000007</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>16</v>
       </c>
@@ -4845,8 +4951,14 @@
       <c r="E19" s="14">
         <v>205823.9</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19">
+        <v>2.4057580000000001</v>
+      </c>
+      <c r="G19" s="27">
+        <v>98.783199999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>17</v>
       </c>
@@ -4862,8 +4974,14 @@
       <c r="E20" s="14">
         <v>202027</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20">
+        <v>2.4018169999999999</v>
+      </c>
+      <c r="G20" s="27">
+        <v>98.789140000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>18</v>
       </c>
@@ -4879,8 +4997,14 @@
       <c r="E21" s="14">
         <v>195067.2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21">
+        <v>2.3980589999999999</v>
+      </c>
+      <c r="G21" s="27">
+        <v>98.793409999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>19</v>
       </c>
@@ -4896,8 +5020,14 @@
       <c r="E22" s="14">
         <v>195775.8</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22">
+        <v>2.3979759999999999</v>
+      </c>
+      <c r="G22" s="27">
+        <v>98.818939999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>20</v>
       </c>
@@ -4913,8 +5043,14 @@
       <c r="E23" s="14">
         <v>198862.8</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23">
+        <v>2.4003589999999999</v>
+      </c>
+      <c r="G23" s="27">
+        <v>98.806129999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>21</v>
       </c>
@@ -4930,8 +5066,14 @@
       <c r="E24" s="14">
         <v>184831.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24">
+        <v>2.3799260000000002</v>
+      </c>
+      <c r="G24" s="27">
+        <v>98.862539999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>22</v>
       </c>
@@ -4947,8 +5089,14 @@
       <c r="E25" s="14">
         <v>185749.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25">
+        <v>2.3938920000000001</v>
+      </c>
+      <c r="G25" s="27">
+        <v>98.822929999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>23</v>
       </c>
@@ -4964,8 +5112,14 @@
       <c r="E26" s="14">
         <v>214886.3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26">
+        <v>2.4104519999999998</v>
+      </c>
+      <c r="G26" s="27">
+        <v>98.758279999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>24</v>
       </c>
@@ -4981,8 +5135,17 @@
       <c r="E27" s="14">
         <v>197173.8</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27">
+        <v>2.3997980000000001</v>
+      </c>
+      <c r="G27" s="27">
+        <v>98.802670000000006</v>
+      </c>
+      <c r="H27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -4992,8 +5155,9 @@
       <c r="E28" s="14">
         <v>133147.79999999999</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28" s="27"/>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -5003,8 +5167,9 @@
       <c r="E29" s="14">
         <v>204300.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29" s="27"/>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -5014,8 +5179,9 @@
       <c r="E30" s="14">
         <v>135118.20000000001</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="G30" s="27"/>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -5025,6 +5191,7 @@
       <c r="E31" s="14">
         <v>203706.5</v>
       </c>
+      <c r="G31" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added EP and SV to FPVA plotting. Plotted min/max against MHR and IHR sufficient summary plots
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26621"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1460" yWindow="1320" windowWidth="25360" windowHeight="15820" activeTab="4"/>
+    <workbookView xWindow="20" yWindow="1080" windowWidth="25360" windowHeight="15820" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ER25" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="84">
   <si>
     <t>ER</t>
   </si>
@@ -272,6 +272,9 @@
   </si>
   <si>
     <t>more…</t>
+  </si>
+  <si>
+    <t>min/max integral computed differently? Weighted?</t>
   </si>
 </sst>
 </file>
@@ -282,7 +285,7 @@
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000E+00"/>
-    <numFmt numFmtId="170" formatCode="0.00000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -352,8 +355,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="59">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -570,6 +621,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -591,11 +645,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="59">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -625,6 +676,14 @@
     <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -654,6 +713,14 @@
     <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1992,20 +2059,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4"/>
@@ -2034,7 +2101,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>0.25</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2056,7 +2123,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2076,7 +2143,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2096,7 +2163,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2116,7 +2183,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2136,7 +2203,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2156,7 +2223,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2176,7 +2243,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2196,7 +2263,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2216,7 +2283,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2236,7 +2303,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2256,7 +2323,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2276,7 +2343,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2296,7 +2363,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2316,7 +2383,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2396,31 +2463,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2446,7 +2513,7 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="25">
+      <c r="A3" s="26">
         <v>0.3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2479,7 +2546,7 @@
       <c r="K3" s="7"/>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -2500,7 +2567,7 @@
       <c r="K4" s="7"/>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -2521,7 +2588,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2542,7 +2609,7 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -2563,7 +2630,7 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -2584,7 +2651,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -2605,7 +2672,7 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -2626,7 +2693,7 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2647,7 +2714,7 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2668,7 +2735,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -2689,7 +2756,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2710,7 +2777,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -2731,7 +2798,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2752,7 +2819,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -3613,31 +3680,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3665,7 +3732,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3690,7 +3757,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -3713,7 +3780,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3736,7 +3803,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -3759,7 +3826,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3782,7 +3849,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -3805,7 +3872,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -3828,7 +3895,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -3849,7 +3916,7 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -3872,7 +3939,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -3895,7 +3962,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -3918,7 +3985,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -3941,7 +4008,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -3964,7 +4031,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -3987,7 +4054,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4096,31 +4163,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="21"/>
+      <c r="J1" s="22"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4148,7 +4215,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="22">
+      <c r="A3" s="23">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4173,7 +4240,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="23"/>
+      <c r="A4" s="24"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4196,7 +4263,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="23"/>
+      <c r="A5" s="24"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4219,7 +4286,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="23"/>
+      <c r="A6" s="24"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -4242,7 +4309,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="23"/>
+      <c r="A7" s="24"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -4265,7 +4332,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="23"/>
+      <c r="A8" s="24"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4288,7 +4355,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="23"/>
+      <c r="A9" s="24"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4311,7 +4378,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="23"/>
+      <c r="A10" s="24"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4334,7 +4401,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="23"/>
+      <c r="A11" s="24"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -4357,7 +4424,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="23"/>
+      <c r="A12" s="24"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -4380,7 +4447,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="23"/>
+      <c r="A13" s="24"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4403,7 +4470,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="23"/>
+      <c r="A14" s="24"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -4426,7 +4493,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="23"/>
+      <c r="A15" s="24"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4449,7 +4516,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="23"/>
+      <c r="A16" s="24"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4472,7 +4539,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="23"/>
+      <c r="A17" s="24"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4516,10 +4583,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4532,18 +4599,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26" t="s">
+      <c r="C1" s="27"/>
+      <c r="D1" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26" t="s">
+      <c r="E1" s="27"/>
+      <c r="F1" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="26"/>
+      <c r="G1" s="27"/>
     </row>
     <row r="2" spans="1:8" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -4583,7 +4650,7 @@
       <c r="F3">
         <v>2.3790249999999999</v>
       </c>
-      <c r="G3" s="27">
+      <c r="G3" s="20">
         <v>98.873630000000006</v>
       </c>
     </row>
@@ -4606,7 +4673,7 @@
       <c r="F4">
         <v>2.3896679999999999</v>
       </c>
-      <c r="G4" s="27">
+      <c r="G4" s="20">
         <v>98.844089999999994</v>
       </c>
     </row>
@@ -4629,7 +4696,7 @@
       <c r="F5">
         <v>2.393329</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="20">
         <v>98.823070000000001</v>
       </c>
     </row>
@@ -4652,7 +4719,7 @@
       <c r="F6">
         <v>2.4024160000000001</v>
       </c>
-      <c r="G6" s="27">
+      <c r="G6" s="20">
         <v>98.806430000000006</v>
       </c>
     </row>
@@ -4675,7 +4742,7 @@
       <c r="F7">
         <v>2.3998360000000001</v>
       </c>
-      <c r="G7" s="27">
+      <c r="G7" s="20">
         <v>98.801029999999997</v>
       </c>
     </row>
@@ -4698,7 +4765,7 @@
       <c r="F8">
         <v>2.3862930000000002</v>
       </c>
-      <c r="G8" s="27">
+      <c r="G8" s="20">
         <v>98.849680000000006</v>
       </c>
     </row>
@@ -4721,7 +4788,7 @@
       <c r="F9">
         <v>2.3887040000000002</v>
       </c>
-      <c r="G9" s="27">
+      <c r="G9" s="20">
         <v>98.832049999999995</v>
       </c>
     </row>
@@ -4744,7 +4811,7 @@
       <c r="F10">
         <v>2.3894449999999998</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="20">
         <v>98.840479999999999</v>
       </c>
     </row>
@@ -4767,7 +4834,7 @@
       <c r="F11">
         <v>2.385821</v>
       </c>
-      <c r="G11" s="27">
+      <c r="G11" s="20">
         <v>98.856620000000007</v>
       </c>
     </row>
@@ -4790,7 +4857,7 @@
       <c r="F12">
         <v>2.4035739999999999</v>
       </c>
-      <c r="G12" s="27">
+      <c r="G12" s="20">
         <v>98.772540000000006</v>
       </c>
     </row>
@@ -4813,7 +4880,7 @@
       <c r="F13">
         <v>2.3931450000000001</v>
       </c>
-      <c r="G13" s="27">
+      <c r="G13" s="20">
         <v>98.813389999999998</v>
       </c>
     </row>
@@ -4836,7 +4903,7 @@
       <c r="F14">
         <v>2.3806240000000001</v>
       </c>
-      <c r="G14" s="27">
+      <c r="G14" s="20">
         <v>98.862359999999995</v>
       </c>
     </row>
@@ -4859,7 +4926,7 @@
       <c r="F15">
         <v>2.4004530000000002</v>
       </c>
-      <c r="G15" s="27">
+      <c r="G15" s="20">
         <v>98.794079999999994</v>
       </c>
     </row>
@@ -4882,7 +4949,7 @@
       <c r="F16">
         <v>2.3944990000000002</v>
       </c>
-      <c r="G16" s="27">
+      <c r="G16" s="20">
         <v>98.821259999999995</v>
       </c>
       <c r="H16" t="s">
@@ -4908,7 +4975,7 @@
       <c r="F17">
         <v>2.388582</v>
       </c>
-      <c r="G17" s="27">
+      <c r="G17" s="20">
         <v>98.828029999999998</v>
       </c>
     </row>
@@ -4931,7 +4998,7 @@
       <c r="F18">
         <v>2.4085960000000002</v>
       </c>
-      <c r="G18" s="27">
+      <c r="G18" s="20">
         <v>98.773750000000007</v>
       </c>
     </row>
@@ -4954,7 +5021,7 @@
       <c r="F19">
         <v>2.4057580000000001</v>
       </c>
-      <c r="G19" s="27">
+      <c r="G19" s="20">
         <v>98.783199999999994</v>
       </c>
     </row>
@@ -4977,7 +5044,7 @@
       <c r="F20">
         <v>2.4018169999999999</v>
       </c>
-      <c r="G20" s="27">
+      <c r="G20" s="20">
         <v>98.789140000000003</v>
       </c>
     </row>
@@ -5000,7 +5067,7 @@
       <c r="F21">
         <v>2.3980589999999999</v>
       </c>
-      <c r="G21" s="27">
+      <c r="G21" s="20">
         <v>98.793409999999994</v>
       </c>
     </row>
@@ -5023,7 +5090,7 @@
       <c r="F22">
         <v>2.3979759999999999</v>
       </c>
-      <c r="G22" s="27">
+      <c r="G22" s="20">
         <v>98.818939999999998</v>
       </c>
     </row>
@@ -5046,7 +5113,7 @@
       <c r="F23">
         <v>2.4003589999999999</v>
       </c>
-      <c r="G23" s="27">
+      <c r="G23" s="20">
         <v>98.806129999999996</v>
       </c>
     </row>
@@ -5069,7 +5136,7 @@
       <c r="F24">
         <v>2.3799260000000002</v>
       </c>
-      <c r="G24" s="27">
+      <c r="G24" s="20">
         <v>98.862539999999996</v>
       </c>
     </row>
@@ -5092,7 +5159,7 @@
       <c r="F25">
         <v>2.3938920000000001</v>
       </c>
-      <c r="G25" s="27">
+      <c r="G25" s="20">
         <v>98.822929999999999</v>
       </c>
     </row>
@@ -5115,7 +5182,7 @@
       <c r="F26">
         <v>2.4104519999999998</v>
       </c>
-      <c r="G26" s="27">
+      <c r="G26" s="20">
         <v>98.758279999999999</v>
       </c>
     </row>
@@ -5138,7 +5205,7 @@
       <c r="F27">
         <v>2.3997980000000001</v>
       </c>
-      <c r="G27" s="27">
+      <c r="G27" s="20">
         <v>98.802670000000006</v>
       </c>
       <c r="H27" t="s">
@@ -5155,7 +5222,7 @@
       <c r="E28" s="14">
         <v>133147.79999999999</v>
       </c>
-      <c r="G28" s="27"/>
+      <c r="G28" s="20"/>
     </row>
     <row r="29" spans="1:8">
       <c r="A29" t="s">
@@ -5167,7 +5234,7 @@
       <c r="E29" s="14">
         <v>204300.5</v>
       </c>
-      <c r="G29" s="27"/>
+      <c r="G29" s="20"/>
     </row>
     <row r="30" spans="1:8">
       <c r="A30" t="s">
@@ -5179,7 +5246,7 @@
       <c r="E30" s="14">
         <v>135118.20000000001</v>
       </c>
-      <c r="G30" s="27"/>
+      <c r="G30" s="20"/>
     </row>
     <row r="31" spans="1:8">
       <c r="A31" t="s">
@@ -5191,7 +5258,12 @@
       <c r="E31" s="14">
         <v>203706.5</v>
       </c>
-      <c r="G31" s="27"/>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:8" ht="64">
+      <c r="E32" t="s">
+        <v>83</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Added additional samples that needed more runtime for convergence
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
   <si>
     <t>ER</t>
   </si>
@@ -269,9 +269,6 @@
   </si>
   <si>
     <t>SupersonicVolume</t>
-  </si>
-  <si>
-    <t>more…</t>
   </si>
   <si>
     <t>min/max integral computed differently? Weighted?</t>
@@ -2446,7 +2443,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A43" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
@@ -4583,10 +4580,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4598,7 +4595,7 @@
     <col min="5" max="5" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:7">
       <c r="B1" s="27" t="s">
         <v>73</v>
       </c>
@@ -4612,7 +4609,7 @@
       </c>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="1:8" s="13" customFormat="1" ht="32">
+    <row r="2" spans="1:7" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
@@ -4635,7 +4632,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:7">
       <c r="A3" s="18" t="s">
         <v>74</v>
       </c>
@@ -4654,7 +4651,7 @@
         <v>98.873630000000006</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4677,7 +4674,7 @@
         <v>98.844089999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4700,7 +4697,7 @@
         <v>98.823070000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4723,7 +4720,7 @@
         <v>98.806430000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4746,7 +4743,7 @@
         <v>98.801029999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4769,7 +4766,7 @@
         <v>98.849680000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4792,7 +4789,7 @@
         <v>98.832049999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4815,7 +4812,7 @@
         <v>98.840479999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4838,7 +4835,7 @@
         <v>98.856620000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4861,7 +4858,7 @@
         <v>98.772540000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4884,7 +4881,7 @@
         <v>98.813389999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4907,7 +4904,7 @@
         <v>98.862359999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4930,7 +4927,7 @@
         <v>98.794079999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>13</v>
       </c>
@@ -4947,16 +4944,13 @@
         <v>188740.6</v>
       </c>
       <c r="F16">
-        <v>2.3944990000000002</v>
+        <v>2.3945959999999999</v>
       </c>
       <c r="G16" s="20">
         <v>98.821259999999995</v>
       </c>
-      <c r="H16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>14</v>
       </c>
@@ -4979,7 +4973,7 @@
         <v>98.828029999999998</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5002,7 +4996,7 @@
         <v>98.773750000000007</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5025,7 +5019,7 @@
         <v>98.783199999999994</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5048,7 +5042,7 @@
         <v>98.789140000000003</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5071,7 +5065,7 @@
         <v>98.793409999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5094,7 +5088,7 @@
         <v>98.818939999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5117,7 +5111,7 @@
         <v>98.806129999999996</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5140,7 +5134,7 @@
         <v>98.862539999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5163,7 +5157,7 @@
         <v>98.822929999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>23</v>
       </c>
@@ -5186,7 +5180,7 @@
         <v>98.758279999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>24</v>
       </c>
@@ -5203,16 +5197,13 @@
         <v>197173.8</v>
       </c>
       <c r="F27">
-        <v>2.3997980000000001</v>
+        <v>2.4003679999999998</v>
       </c>
       <c r="G27" s="20">
-        <v>98.802670000000006</v>
-      </c>
-      <c r="H27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
+        <v>98.801169999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>75</v>
       </c>
@@ -5224,7 +5215,7 @@
       </c>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>76</v>
       </c>
@@ -5236,7 +5227,7 @@
       </c>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -5248,7 +5239,7 @@
       </c>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>78</v>
       </c>
@@ -5260,9 +5251,9 @@
       </c>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="1:8" ht="64">
+    <row r="32" spans="1:7" ht="64">
       <c r="E32" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added other FFR 1iter results and AS post processing.
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -4,14 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="1080" windowWidth="25360" windowHeight="15820" activeTab="4"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="25360" windowHeight="15820" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="ER25" sheetId="1" r:id="rId1"/>
     <sheet name="ER30" sheetId="2" r:id="rId2"/>
     <sheet name="ER35" sheetId="3" r:id="rId3"/>
     <sheet name="ER40" sheetId="4" r:id="rId4"/>
-    <sheet name="FPVA" sheetId="5" r:id="rId5"/>
+    <sheet name="FPVA25" sheetId="6" r:id="rId5"/>
+    <sheet name="FPVA30" sheetId="5" r:id="rId6"/>
+    <sheet name="FPVA35" sheetId="7" r:id="rId7"/>
+    <sheet name="FPVA40" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="88">
   <si>
     <t>ER</t>
   </si>
@@ -272,6 +275,21 @@
   </si>
   <si>
     <t>min/max integral computed differently? Weighted?</t>
+  </si>
+  <si>
+    <t>P range:</t>
+  </si>
+  <si>
+    <t>SV range:</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Range:</t>
   </si>
 </sst>
 </file>
@@ -352,7 +370,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="75">
+  <cellStyleXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -578,8 +596,74 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -642,8 +726,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="75">
+  <cellStyles count="97">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -681,6 +771,17 @@
     <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -718,6 +819,17 @@
     <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2443,8 +2555,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -2456,10 +2568,12 @@
     <col min="7" max="7" width="10.375" style="5" customWidth="1"/>
     <col min="8" max="8" width="10.625" style="5" customWidth="1"/>
     <col min="9" max="10" width="10.375" style="5" customWidth="1"/>
-    <col min="11" max="256" width="9.375" style="5" customWidth="1"/>
+    <col min="11" max="12" width="9.375" style="5" customWidth="1"/>
+    <col min="13" max="14" width="12.125" style="5" customWidth="1"/>
+    <col min="15" max="256" width="9.375" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="19" customHeight="1">
+    <row r="1" spans="1:14" ht="19" customHeight="1">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -2482,7 +2596,7 @@
       <c r="J1" s="22"/>
       <c r="K1" s="7"/>
     </row>
-    <row r="2" spans="1:11" ht="19" customHeight="1">
+    <row r="2" spans="1:14" ht="19" customHeight="1">
       <c r="A2" s="22"/>
       <c r="B2" s="22"/>
       <c r="C2" s="7" t="s">
@@ -2509,7 +2623,7 @@
       </c>
       <c r="K2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="19" customHeight="1">
+    <row r="3" spans="1:14" ht="19" customHeight="1">
       <c r="A3" s="26">
         <v>0.3</v>
       </c>
@@ -2541,8 +2655,19 @@
         <v>98.873410000000007</v>
       </c>
       <c r="K3" s="7"/>
-    </row>
-    <row r="4" spans="1:11" ht="19" customHeight="1">
+      <c r="L3" t="s">
+        <v>83</v>
+      </c>
+      <c r="M3" s="20">
+        <f>MIN($I4:$I55)</f>
+        <v>2.0861079999999999</v>
+      </c>
+      <c r="N3" s="20">
+        <f>MAX($I4:$I55)</f>
+        <v>2.7295280000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="19" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="6" t="s">
         <v>13</v>
@@ -2562,8 +2687,19 @@
         <v>99.003320000000002</v>
       </c>
       <c r="K4" s="7"/>
-    </row>
-    <row r="5" spans="1:11" ht="19" customHeight="1">
+      <c r="L4" t="s">
+        <v>84</v>
+      </c>
+      <c r="M4" s="28">
+        <f>MIN($J4:$J55)</f>
+        <v>98.346900000000005</v>
+      </c>
+      <c r="N4" s="28">
+        <f>MAX($J4:$J55)</f>
+        <v>99.157799999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="19" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
@@ -2584,7 +2720,7 @@
       </c>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" ht="19" customHeight="1">
+    <row r="6" spans="1:14" ht="19" customHeight="1">
       <c r="A6" s="24"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
@@ -2605,7 +2741,7 @@
       </c>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="19" customHeight="1">
+    <row r="7" spans="1:14" ht="19" customHeight="1">
       <c r="A7" s="24"/>
       <c r="B7" s="6" t="s">
         <v>16</v>
@@ -2626,7 +2762,7 @@
       </c>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" ht="19" customHeight="1">
+    <row r="8" spans="1:14" ht="19" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
@@ -2647,7 +2783,7 @@
       </c>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" ht="19" customHeight="1">
+    <row r="9" spans="1:14" ht="19" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
@@ -2668,7 +2804,7 @@
       </c>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" ht="19" customHeight="1">
+    <row r="10" spans="1:14" ht="19" customHeight="1">
       <c r="A10" s="24"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
@@ -2689,7 +2825,7 @@
       </c>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" ht="19" customHeight="1">
+    <row r="11" spans="1:14" ht="19" customHeight="1">
       <c r="A11" s="24"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
@@ -2710,7 +2846,7 @@
       </c>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" ht="19" customHeight="1">
+    <row r="12" spans="1:14" ht="19" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
@@ -2731,7 +2867,7 @@
       </c>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" ht="19" customHeight="1">
+    <row r="13" spans="1:14" ht="19" customHeight="1">
       <c r="A13" s="24"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
@@ -2752,7 +2888,7 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" ht="19" customHeight="1">
+    <row r="14" spans="1:14" ht="19" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="6" t="s">
         <v>23</v>
@@ -2773,7 +2909,7 @@
       </c>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" ht="19" customHeight="1">
+    <row r="15" spans="1:14" ht="19" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="6" t="s">
         <v>24</v>
@@ -2794,7 +2930,7 @@
       </c>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" ht="19" customHeight="1">
+    <row r="16" spans="1:14" ht="19" customHeight="1">
       <c r="A16" s="24"/>
       <c r="B16" s="6" t="s">
         <v>25</v>
@@ -4580,10 +4716,395 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="8" max="9" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
+      <c r="A2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14">
+        <v>209543000000</v>
+      </c>
+      <c r="C4" s="29">
+        <v>154147.5</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14">
+        <v>218537000000</v>
+      </c>
+      <c r="C5" s="14">
+        <v>166467.79999999999</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14">
+        <v>225695000000</v>
+      </c>
+      <c r="C6" s="14">
+        <v>168527.9</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14">
+        <v>247187000000</v>
+      </c>
+      <c r="C7" s="14">
+        <v>163965.29999999999</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14">
+        <v>203189000000</v>
+      </c>
+      <c r="C8" s="14">
+        <v>157435</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14">
+        <v>239773000000</v>
+      </c>
+      <c r="C9" s="14">
+        <v>151547.29999999999</v>
+      </c>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14">
+        <v>209532000000</v>
+      </c>
+      <c r="C10" s="14">
+        <v>163405.1</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14">
+        <v>195636000000</v>
+      </c>
+      <c r="C11" s="14">
+        <v>158033.70000000001</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>247692000000</v>
+      </c>
+      <c r="C12" s="14">
+        <v>172006.1</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="14">
+        <v>236010000000</v>
+      </c>
+      <c r="C13" s="14">
+        <v>157523.20000000001</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14">
+        <v>201018000000</v>
+      </c>
+      <c r="C14" s="14">
+        <v>147609.4</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="14">
+        <v>246948000000</v>
+      </c>
+      <c r="C15" s="14">
+        <v>166012</v>
+      </c>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="14">
+        <v>221769000000</v>
+      </c>
+      <c r="C16" s="14">
+        <v>159644.9</v>
+      </c>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14">
+        <v>229203000000</v>
+      </c>
+      <c r="C17" s="14">
+        <v>152564</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14">
+        <v>236624000000</v>
+      </c>
+      <c r="C18" s="14">
+        <v>178583.2</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14">
+        <v>235324000000</v>
+      </c>
+      <c r="C19" s="14">
+        <v>174084.6</v>
+      </c>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14">
+        <v>234909000000</v>
+      </c>
+      <c r="C20" s="14">
+        <v>170636.79999999999</v>
+      </c>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14">
+        <v>237980000000</v>
+      </c>
+      <c r="C21" s="14">
+        <v>164753.20000000001</v>
+      </c>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14">
+        <v>214693000000</v>
+      </c>
+      <c r="C22" s="14">
+        <v>165835.29999999999</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14">
+        <v>223315000000</v>
+      </c>
+      <c r="C23" s="14">
+        <v>168006.2</v>
+      </c>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="14">
+        <v>204919000000</v>
+      </c>
+      <c r="C24" s="14">
+        <v>157026.29999999999</v>
+      </c>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="14">
+        <v>245784000000</v>
+      </c>
+      <c r="C25" s="14">
+        <v>156623.79999999999</v>
+      </c>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="14">
+        <v>251214000000</v>
+      </c>
+      <c r="C26" s="14">
+        <v>181974.1</v>
+      </c>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="14">
+        <v>239258000000</v>
+      </c>
+      <c r="C27" s="14">
+        <v>166408.79999999999</v>
+      </c>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="14">
+        <f>MIN(B$4:B$27)</f>
+        <v>195636000000</v>
+      </c>
+      <c r="C30" s="14">
+        <f>MIN(C$4:C$27)</f>
+        <v>147609.4</v>
+      </c>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="14">
+        <f>MAX(B$4:B$27)</f>
+        <v>251214000000</v>
+      </c>
+      <c r="C31" s="14">
+        <f>MAX(C$4:C$27)</f>
+        <v>181974.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -4593,9 +5114,10 @@
     <col min="3" max="3" width="17.375" customWidth="1"/>
     <col min="4" max="4" width="11.25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.875" customWidth="1"/>
+    <col min="10" max="11" width="11.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:11">
       <c r="B1" s="27" t="s">
         <v>73</v>
       </c>
@@ -4609,7 +5131,7 @@
       </c>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="1:7" s="13" customFormat="1" ht="32">
+    <row r="2" spans="1:11" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
         <v>66</v>
       </c>
@@ -4632,7 +5154,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:11">
       <c r="A3" s="18" t="s">
         <v>74</v>
       </c>
@@ -4650,8 +5172,19 @@
       <c r="G3" s="20">
         <v>98.873630000000006</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3">
+        <f>MIN($F4:$F27)</f>
+        <v>2.3799260000000002</v>
+      </c>
+      <c r="K3">
+        <f>MAX($F4:$F27)</f>
+        <v>2.4104519999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4673,8 +5206,19 @@
       <c r="G4" s="20">
         <v>98.844089999999994</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" t="s">
+        <v>84</v>
+      </c>
+      <c r="J4" s="28">
+        <f>MIN($G5:$G28)</f>
+        <v>98.758279999999999</v>
+      </c>
+      <c r="K4" s="28">
+        <f>MAX($G5:$G28)</f>
+        <v>98.862539999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4697,7 +5241,7 @@
         <v>98.823070000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4720,7 +5264,7 @@
         <v>98.806430000000006</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:11">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4743,7 +5287,7 @@
         <v>98.801029999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:11">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4766,7 +5310,7 @@
         <v>98.849680000000006</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:11">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4789,7 +5333,7 @@
         <v>98.832049999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:11">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4812,7 +5356,7 @@
         <v>98.840479999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:11">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4835,7 +5379,7 @@
         <v>98.856620000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:11">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4858,7 +5402,7 @@
         <v>98.772540000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:11">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4881,7 +5425,7 @@
         <v>98.813389999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:11">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4904,7 +5448,7 @@
         <v>98.862359999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:11">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4927,7 +5471,7 @@
         <v>98.794079999999994</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:11">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5270,4 +5814,774 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="8" max="9" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
+      <c r="A2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14">
+        <v>215737000000</v>
+      </c>
+      <c r="C4" s="29">
+        <v>198617.60000000001</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14">
+        <v>235519000000</v>
+      </c>
+      <c r="C5" s="14">
+        <v>214574.3</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14">
+        <v>228821000000</v>
+      </c>
+      <c r="C6" s="14">
+        <v>216575.2</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14">
+        <v>252654000000</v>
+      </c>
+      <c r="C7" s="14">
+        <v>211025.4</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14">
+        <v>220146000000</v>
+      </c>
+      <c r="C8" s="14">
+        <v>202914.6</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14">
+        <v>245737000000</v>
+      </c>
+      <c r="C9" s="14">
+        <v>196456.5</v>
+      </c>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14">
+        <v>225573000000</v>
+      </c>
+      <c r="C10" s="14">
+        <v>209589.1</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14">
+        <v>212363000000</v>
+      </c>
+      <c r="C11" s="14">
+        <v>203864.3</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>263673000000</v>
+      </c>
+      <c r="C12" s="14">
+        <v>221152.9</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="14">
+        <v>244073000000</v>
+      </c>
+      <c r="C13" s="14">
+        <v>203214.7</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14">
+        <v>213464000000</v>
+      </c>
+      <c r="C14" s="14">
+        <v>191133.3</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="14">
+        <v>253492000000</v>
+      </c>
+      <c r="C15" s="14">
+        <v>213669.8</v>
+      </c>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="14">
+        <v>228177000000</v>
+      </c>
+      <c r="C16" s="14">
+        <v>205549.3</v>
+      </c>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14">
+        <v>236594000000</v>
+      </c>
+      <c r="C17" s="14">
+        <v>197338.3</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14">
+        <v>251590000000</v>
+      </c>
+      <c r="C18" s="14">
+        <v>229204.8</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14">
+        <v>249405000000</v>
+      </c>
+      <c r="C19" s="14">
+        <v>223770.3</v>
+      </c>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14">
+        <v>252038000000</v>
+      </c>
+      <c r="C20" s="14">
+        <v>220011.9</v>
+      </c>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14">
+        <v>254208000000</v>
+      </c>
+      <c r="C21" s="14">
+        <v>212403.9</v>
+      </c>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14">
+        <v>222196000000</v>
+      </c>
+      <c r="C22" s="14">
+        <v>213135.8</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14">
+        <v>232320000000</v>
+      </c>
+      <c r="C23" s="14">
+        <v>216544.3</v>
+      </c>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="14">
+        <v>220232000000</v>
+      </c>
+      <c r="C24" s="14">
+        <v>201386.9</v>
+      </c>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="14">
+        <v>252165000000</v>
+      </c>
+      <c r="C25" s="14">
+        <v>202580.2</v>
+      </c>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="14">
+        <v>267270000000</v>
+      </c>
+      <c r="C26" s="14">
+        <v>233287.1</v>
+      </c>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="14">
+        <v>244563000000</v>
+      </c>
+      <c r="C27" s="14">
+        <v>214793.2</v>
+      </c>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="14">
+        <f>MIN(B$4:B$27)</f>
+        <v>212363000000</v>
+      </c>
+      <c r="C30" s="14">
+        <f>MIN(C$4:C$27)</f>
+        <v>191133.3</v>
+      </c>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="14">
+        <f>MAX(B$4:B$27)</f>
+        <v>267270000000</v>
+      </c>
+      <c r="C31" s="14">
+        <f>MAX(C$4:C$27)</f>
+        <v>233287.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="11.25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" customWidth="1"/>
+    <col min="8" max="9" width="11.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="B1" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+    </row>
+    <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
+      <c r="A2" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" s="14">
+        <v>212836000000</v>
+      </c>
+      <c r="C4" s="29">
+        <v>219897.5</v>
+      </c>
+      <c r="E4" s="20"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="14">
+        <v>228429000000</v>
+      </c>
+      <c r="C5" s="14">
+        <v>236457.8</v>
+      </c>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="14">
+        <v>226636000000</v>
+      </c>
+      <c r="C6" s="14">
+        <v>238661.5</v>
+      </c>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14">
+        <v>252700000000</v>
+      </c>
+      <c r="C7" s="14">
+        <v>233334.3</v>
+      </c>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="14">
+        <v>213104000000</v>
+      </c>
+      <c r="C8" s="14">
+        <v>223758.2</v>
+      </c>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9">
+        <v>6</v>
+      </c>
+      <c r="B9" s="14">
+        <v>245872000000</v>
+      </c>
+      <c r="C9" s="14">
+        <v>218434.7</v>
+      </c>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10">
+        <v>7</v>
+      </c>
+      <c r="B10" s="14">
+        <v>219754000000</v>
+      </c>
+      <c r="C10" s="14">
+        <v>230324.5</v>
+      </c>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" s="14">
+        <v>205002000000</v>
+      </c>
+      <c r="C11" s="14">
+        <v>224343.7</v>
+      </c>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12" s="14">
+        <v>258548000000</v>
+      </c>
+      <c r="C12" s="14">
+        <v>244065.2</v>
+      </c>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13">
+        <v>10</v>
+      </c>
+      <c r="B13" s="14">
+        <v>240482000000</v>
+      </c>
+      <c r="C13" s="14">
+        <v>225331.8</v>
+      </c>
+      <c r="E13" s="20"/>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14">
+        <v>207509000000</v>
+      </c>
+      <c r="C14" s="14">
+        <v>212230.8</v>
+      </c>
+      <c r="E14" s="20"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15">
+        <v>12</v>
+      </c>
+      <c r="B15" s="14">
+        <v>254287000000</v>
+      </c>
+      <c r="C15" s="14">
+        <v>236155.9</v>
+      </c>
+      <c r="E15" s="20"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16">
+        <v>13</v>
+      </c>
+      <c r="B16" s="14">
+        <v>225475000000</v>
+      </c>
+      <c r="C16" s="14">
+        <v>227463.6</v>
+      </c>
+      <c r="E16" s="20"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>14</v>
+      </c>
+      <c r="B17" s="14">
+        <v>232940000000</v>
+      </c>
+      <c r="C17" s="14">
+        <v>219300.2</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>15</v>
+      </c>
+      <c r="B18" s="14">
+        <v>247386000000</v>
+      </c>
+      <c r="C18" s="14">
+        <v>251947.7</v>
+      </c>
+      <c r="E18" s="20"/>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>16</v>
+      </c>
+      <c r="B19" s="14">
+        <v>245138000000</v>
+      </c>
+      <c r="C19" s="14">
+        <v>246441.2</v>
+      </c>
+      <c r="E19" s="20"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>17</v>
+      </c>
+      <c r="B20" s="14">
+        <v>245242000000</v>
+      </c>
+      <c r="C20" s="14">
+        <v>242721.2</v>
+      </c>
+      <c r="E20" s="20"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
+        <v>18</v>
+      </c>
+      <c r="B21" s="14">
+        <v>248241000000</v>
+      </c>
+      <c r="C21" s="14">
+        <v>235001.8</v>
+      </c>
+      <c r="E21" s="20"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>19</v>
+      </c>
+      <c r="B22" s="14">
+        <v>220043000000</v>
+      </c>
+      <c r="C22" s="14">
+        <v>234984.8</v>
+      </c>
+      <c r="E22" s="20"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23">
+        <v>20</v>
+      </c>
+      <c r="B23" s="14">
+        <v>228447000000</v>
+      </c>
+      <c r="C23" s="14">
+        <v>238802.1</v>
+      </c>
+      <c r="E23" s="20"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24">
+        <v>21</v>
+      </c>
+      <c r="B24" s="14">
+        <v>214554000000</v>
+      </c>
+      <c r="C24" s="14">
+        <v>220850.8</v>
+      </c>
+      <c r="E24" s="20"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25">
+        <v>22</v>
+      </c>
+      <c r="B25" s="14">
+        <v>252658000000</v>
+      </c>
+      <c r="C25" s="14">
+        <v>224625.4</v>
+      </c>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26">
+        <v>23</v>
+      </c>
+      <c r="B26" s="14">
+        <v>263216000000</v>
+      </c>
+      <c r="C26" s="14">
+        <v>256216.8</v>
+      </c>
+      <c r="E26" s="20"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27">
+        <v>24</v>
+      </c>
+      <c r="B27" s="14">
+        <v>244534000000</v>
+      </c>
+      <c r="C27" s="14">
+        <v>237321.3</v>
+      </c>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>87</v>
+      </c>
+      <c r="E29" s="20"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="14">
+        <f>MIN(B$4:B$27)</f>
+        <v>205002000000</v>
+      </c>
+      <c r="C30" s="14">
+        <f>MIN(C$4:C$27)</f>
+        <v>212230.8</v>
+      </c>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="B31" s="14">
+        <f>MAX(B$4:B$27)</f>
+        <v>263216000000</v>
+      </c>
+      <c r="C31" s="14">
+        <f>MAX(C$4:C$27)</f>
+        <v>256216.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added turbulence only 3D results, full system QMU comparisons for all FFRs
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -4,17 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="25360" windowHeight="15820" activeTab="7"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="11"/>
   </bookViews>
   <sheets>
-    <sheet name="ER25" sheetId="1" r:id="rId1"/>
-    <sheet name="ER30" sheetId="2" r:id="rId2"/>
-    <sheet name="ER35" sheetId="3" r:id="rId3"/>
-    <sheet name="ER40" sheetId="4" r:id="rId4"/>
+    <sheet name="inflow25" sheetId="1" r:id="rId1"/>
+    <sheet name="inflow30" sheetId="2" r:id="rId2"/>
+    <sheet name="inflow35" sheetId="3" r:id="rId3"/>
+    <sheet name="inflow40" sheetId="4" r:id="rId4"/>
     <sheet name="FPVA25" sheetId="6" r:id="rId5"/>
     <sheet name="FPVA30" sheetId="5" r:id="rId6"/>
     <sheet name="FPVA35" sheetId="7" r:id="rId7"/>
     <sheet name="FPVA40" sheetId="8" r:id="rId8"/>
+    <sheet name="FFR25" sheetId="10" r:id="rId9"/>
+    <sheet name="FFR30" sheetId="9" r:id="rId10"/>
+    <sheet name="FFR35" sheetId="11" r:id="rId11"/>
+    <sheet name="FFR40" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="107">
   <si>
     <t>ER</t>
   </si>
@@ -290,17 +294,75 @@
   </si>
   <si>
     <t xml:space="preserve"> Range:</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>inflow MAX</t>
+  </si>
+  <si>
+    <t>turb MAX</t>
+  </si>
+  <si>
+    <t>FPVA MAX</t>
+  </si>
+  <si>
+    <t>QMU MAX</t>
+  </si>
+  <si>
+    <t>Exit(P)</t>
+  </si>
+  <si>
+    <t>Subsonic Volume</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>linear sum:</t>
+  </si>
+  <si>
+    <t>turb &amp; inflow</t>
+  </si>
+  <si>
+    <t>at what iters should we compare?</t>
+  </si>
+  <si>
+    <t>unstart - no convergence</t>
+  </si>
+  <si>
+    <t>no - steady state</t>
+  </si>
+  <si>
+    <t>rising - not converged</t>
+  </si>
+  <si>
+    <t>still increasing</t>
+  </si>
+  <si>
+    <t>45k iters</t>
+  </si>
+  <si>
+    <t>62k iters</t>
+  </si>
+  <si>
+    <t>60k iters</t>
+  </si>
+  <si>
+    <t>65k iters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.00000E+00"/>
     <numFmt numFmtId="165" formatCode="0.0000E+00"/>
     <numFmt numFmtId="166" formatCode="0.000000E+00"/>
     <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -370,7 +432,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="97">
+  <cellStyleXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -662,8 +724,62 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -705,6 +821,16 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -726,14 +852,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="97">
+  <cellStyles count="115">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -782,6 +905,15 @@
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -830,6 +962,15 @@
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2150,7 +2291,7 @@
   <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -2168,20 +2309,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="26"/>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4"/>
@@ -2210,7 +2351,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="27">
         <v>0.25</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2232,7 +2373,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2252,7 +2393,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2272,7 +2413,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2292,7 +2433,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2312,7 +2453,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2332,7 +2473,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2352,7 +2493,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2372,7 +2513,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2392,7 +2533,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2412,7 +2553,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2432,7 +2573,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2452,7 +2593,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2472,7 +2613,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2492,7 +2633,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2516,8 +2657,12 @@
         <v>69</v>
       </c>
       <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
+      <c r="I18" s="17">
+        <v>2.4634809999999998</v>
+      </c>
+      <c r="J18" s="17">
+        <v>98.685929999999999</v>
+      </c>
     </row>
     <row r="19" spans="1:10" ht="15" customHeight="1">
       <c r="B19" s="1" t="s">
@@ -2551,12 +2696,538 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="32">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="24">
+        <f>inflow30!I3</f>
+        <v>2.3790680000000002</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24">
+        <f>inflow30!J3</f>
+        <v>98.873410000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="24">
+        <f>inflow30!I55</f>
+        <v>2.7295280000000002</v>
+      </c>
+      <c r="C3" s="24">
+        <f>$B3-$B$2</f>
+        <v>0.35045999999999999</v>
+      </c>
+      <c r="D3" s="24">
+        <f>inflow30!J55</f>
+        <v>98.34845</v>
+      </c>
+      <c r="E3" s="23">
+        <f>$D3-$D$2</f>
+        <v>-0.5249600000000072</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>2.7585250000000001</v>
+      </c>
+      <c r="C4" s="24">
+        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <v>0.37945699999999993</v>
+      </c>
+      <c r="D4" s="32">
+        <v>97.968720000000005</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <v>-0.90469000000000221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="23">
+        <f>FPVA30!F29</f>
+        <v>2.4043130000000001</v>
+      </c>
+      <c r="C5" s="24">
+        <f t="shared" si="0"/>
+        <v>2.5244999999999962E-2</v>
+      </c>
+      <c r="D5" s="23">
+        <f>FPVA30!G29</f>
+        <v>98.744730000000004</v>
+      </c>
+      <c r="E5" s="23">
+        <f t="shared" si="1"/>
+        <v>-0.12868000000000279</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="23">
+        <v>3.2817949999999998</v>
+      </c>
+      <c r="C7" s="23">
+        <f>B7-B3</f>
+        <v>0.55226699999999962</v>
+      </c>
+      <c r="D7" s="23">
+        <v>97.108580000000003</v>
+      </c>
+      <c r="E7" s="23">
+        <f>D7-D3</f>
+        <v>-1.2398699999999963</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="23">
+        <f>B2+C9</f>
+        <v>3.1342300000000001</v>
+      </c>
+      <c r="C9" s="23">
+        <f>SUM(C3:C5)</f>
+        <v>0.75516199999999989</v>
+      </c>
+      <c r="D9" s="23">
+        <f>D2+E9</f>
+        <v>97.315079999999995</v>
+      </c>
+      <c r="E9" s="23">
+        <f>SUM(E3:E5)</f>
+        <v>-1.5583300000000122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="23">
+        <v>3.3266170000000002</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23">
+        <v>96.890640000000005</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="32.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="24">
+        <f>inflow35!I3</f>
+        <v>2.6663899999999998</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24">
+        <f>inflow35!J3</f>
+        <v>98.606200000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="24">
+        <f>inflow35!I19</f>
+        <v>3.1274190000000002</v>
+      </c>
+      <c r="C3" s="24">
+        <f>$B3-$B$2</f>
+        <v>0.46102900000000036</v>
+      </c>
+      <c r="D3" s="24">
+        <f>inflow35!J19</f>
+        <v>97.636030000000005</v>
+      </c>
+      <c r="E3" s="23">
+        <f>$D3-$D$2</f>
+        <v>-0.97016999999999598</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>3.2154500000000001</v>
+      </c>
+      <c r="C4" s="24">
+        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <v>0.54906000000000033</v>
+      </c>
+      <c r="D4" s="32">
+        <v>97.129900000000006</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <v>-1.4762999999999948</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="23">
+        <f>inflow35!I20</f>
+        <v>4.3184699999999996</v>
+      </c>
+      <c r="C7" s="23">
+        <f>B7-B2</f>
+        <v>1.6520799999999998</v>
+      </c>
+      <c r="D7" s="23">
+        <f>inflow35!J20</f>
+        <v>87.971599999999995</v>
+      </c>
+      <c r="E7" s="23">
+        <f>D7-D2</f>
+        <v>-10.634600000000006</v>
+      </c>
+      <c r="F7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="23">
+        <f>B2+C9</f>
+        <v>3.6764790000000005</v>
+      </c>
+      <c r="C9" s="23">
+        <f>SUM(C3:C5)</f>
+        <v>1.0100890000000007</v>
+      </c>
+      <c r="D9" s="23">
+        <f>D2+E9</f>
+        <v>96.15973000000001</v>
+      </c>
+      <c r="E9" s="23">
+        <f>SUM(E3:E5)</f>
+        <v>-2.4464699999999908</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="23">
+        <v>4.2274500000000002</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23">
+        <v>90.417199999999994</v>
+      </c>
+      <c r="F10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="6" max="6" width="32.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="32">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="24">
+        <f>inflow40!I3</f>
+        <v>2.9952899999999998</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24">
+        <f>inflow40!J3</f>
+        <v>97.958699999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="24">
+        <f>inflow40!I18</f>
+        <v>3.46618</v>
+      </c>
+      <c r="C3" s="24">
+        <f>$B3-$B$2</f>
+        <v>0.47089000000000025</v>
+      </c>
+      <c r="D3" s="24">
+        <f>inflow40!J18</f>
+        <v>91.628299999999996</v>
+      </c>
+      <c r="E3" s="23">
+        <f>$D3-$D$2</f>
+        <v>-6.3303999999999974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>4.0520500000000004</v>
+      </c>
+      <c r="C4" s="24">
+        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <v>1.0567600000000006</v>
+      </c>
+      <c r="D4" s="32">
+        <v>89.291499999999999</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <v>-8.667199999999994</v>
+      </c>
+      <c r="F4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="23">
+        <f>inflow40!I19</f>
+        <v>4.0458400000000001</v>
+      </c>
+      <c r="C7" s="23">
+        <f>B7-B2</f>
+        <v>1.0505500000000003</v>
+      </c>
+      <c r="D7" s="23">
+        <f>inflow40!J19</f>
+        <v>69.643500000000003</v>
+      </c>
+      <c r="E7" s="23">
+        <f>D7-D2</f>
+        <v>-28.31519999999999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="23">
+        <f>B2+C9</f>
+        <v>4.5229400000000002</v>
+      </c>
+      <c r="C9" s="23">
+        <f>SUM(C3:C5)</f>
+        <v>1.5276500000000008</v>
+      </c>
+      <c r="D9" s="23">
+        <f>D2+E9</f>
+        <v>82.961100000000002</v>
+      </c>
+      <c r="E9" s="23">
+        <f>SUM(E3:E5)</f>
+        <v>-14.997599999999991</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="23">
+        <v>4.0589599999999999</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23">
+        <v>69.544300000000007</v>
+      </c>
+      <c r="F10" t="s">
+        <v>106</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:IV55"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I55" sqref="I55:J55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -2574,31 +3245,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="19" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -2624,7 +3295,7 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="19" customHeight="1">
-      <c r="A3" s="26">
+      <c r="A3" s="30">
         <v>0.3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -2668,7 +3339,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -2690,17 +3361,17 @@
       <c r="L4" t="s">
         <v>84</v>
       </c>
-      <c r="M4" s="28">
+      <c r="M4" s="21">
         <f>MIN($J4:$J55)</f>
         <v>98.346900000000005</v>
       </c>
-      <c r="N4" s="28">
+      <c r="N4" s="21">
         <f>MAX($J4:$J55)</f>
         <v>99.157799999999995</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -2721,7 +3392,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -2742,7 +3413,7 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:14" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -2763,7 +3434,7 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -2784,7 +3455,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -2805,7 +3476,7 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -2826,7 +3497,7 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -2847,7 +3518,7 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -2868,7 +3539,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -2889,7 +3560,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:14" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -2910,7 +3581,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -2931,7 +3602,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -2952,7 +3623,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -3781,6 +4452,7 @@
     <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
     <oddFooter>&amp;L&amp;"Helvetica,Regular"&amp;12&amp;K000000	&amp;P</oddFooter>
   </headerFooter>
@@ -3797,7 +4469,7 @@
   <dimension ref="A1:IV20"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -3813,31 +4485,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -3865,7 +4537,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="27">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -3890,7 +4562,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -3913,7 +4585,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -3936,7 +4608,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -3959,7 +4631,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -3982,7 +4654,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4005,7 +4677,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4028,7 +4700,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4049,7 +4721,7 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -4072,7 +4744,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -4095,7 +4767,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4118,7 +4790,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -4141,7 +4813,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4164,7 +4836,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4187,7 +4859,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4249,10 +4921,22 @@
       <c r="J19" s="9">
         <v>97.636030000000005</v>
       </c>
+      <c r="K19" s="11" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1">
       <c r="B20" s="11" t="s">
         <v>70</v>
+      </c>
+      <c r="I20" s="23">
+        <v>4.3184699999999996</v>
+      </c>
+      <c r="J20" s="11">
+        <v>87.971599999999995</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -4277,10 +4961,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV17"/>
+  <dimension ref="A1:IV19"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H17"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -4296,31 +4980,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="22"/>
+      <c r="J1" s="26"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4348,7 +5032,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="23">
+      <c r="A3" s="27">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4373,7 +5057,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="24"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4396,7 +5080,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="24"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4419,7 +5103,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="24"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -4442,7 +5126,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="24"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -4465,7 +5149,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="24"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4488,7 +5172,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="24"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4511,7 +5195,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="24"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4534,7 +5218,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="24"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -4557,7 +5241,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="24"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -4580,7 +5264,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="24"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4603,7 +5287,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="24"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -4626,7 +5310,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="24"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4649,7 +5333,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="24"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4671,8 +5355,8 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="24"/>
+    <row r="17" spans="1:12" ht="19" customHeight="1">
+      <c r="A17" s="28"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4692,6 +5376,37 @@
       </c>
       <c r="K17" s="2" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15" customHeight="1">
+      <c r="B18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" s="12">
+        <v>3.46618</v>
+      </c>
+      <c r="J18" s="12">
+        <v>91.628299999999996</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="15" customHeight="1">
+      <c r="B19" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="I19" s="12">
+        <v>4.0458400000000001</v>
+      </c>
+      <c r="J19" s="12">
+        <v>69.643500000000003</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -4731,12 +5446,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -4763,12 +5478,12 @@
       <c r="B4" s="14">
         <v>209543000000</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="22">
         <v>154147.5</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
@@ -5104,7 +5819,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -5118,18 +5833,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27" t="s">
+      <c r="E1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="27"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:11" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -5209,13 +5924,13 @@
       <c r="I4" t="s">
         <v>84</v>
       </c>
-      <c r="J4" s="28">
+      <c r="J4" s="21">
         <f>MIN($G5:$G28)</f>
         <v>98.758279999999999</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="21">
         <f>MAX($G5:$G28)</f>
-        <v>98.862539999999996</v>
+        <v>99.003579999999999</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -5757,7 +6472,12 @@
       <c r="E28" s="14">
         <v>133147.79999999999</v>
       </c>
-      <c r="G28" s="20"/>
+      <c r="F28">
+        <v>2.3694459999999999</v>
+      </c>
+      <c r="G28" s="20">
+        <v>99.003579999999999</v>
+      </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
@@ -5769,7 +6489,12 @@
       <c r="E29" s="14">
         <v>204300.5</v>
       </c>
-      <c r="G29" s="20"/>
+      <c r="F29">
+        <v>2.4043130000000001</v>
+      </c>
+      <c r="G29" s="20">
+        <v>98.744730000000004</v>
+      </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
@@ -5793,7 +6518,12 @@
       <c r="E31" s="14">
         <v>203706.5</v>
       </c>
-      <c r="G31" s="20"/>
+      <c r="F31">
+        <v>2.4041779999999999</v>
+      </c>
+      <c r="G31" s="20">
+        <v>98.754980000000003</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="64">
       <c r="E32" t="s">
@@ -5833,12 +6563,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -5865,12 +6595,12 @@
       <c r="B4" s="14">
         <v>215737000000</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="22">
         <v>198617.60000000001</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
@@ -6205,8 +6935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -6218,12 +6948,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -6250,12 +6980,12 @@
       <c r="B4" s="14">
         <v>212836000000</v>
       </c>
-      <c r="C4" s="29">
+      <c r="C4" s="22">
         <v>219897.5</v>
       </c>
       <c r="E4" s="20"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="1:9">
       <c r="A5">
@@ -6584,4 +7314,169 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="32">
+      <c r="A1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="24">
+        <f>inflow25!I3</f>
+        <v>2.1668069999999999</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24">
+        <f>inflow25!J3</f>
+        <v>98.983019999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="24">
+        <f>inflow25!I18</f>
+        <v>2.4634809999999998</v>
+      </c>
+      <c r="C3" s="24">
+        <f>$B3-$B$2</f>
+        <v>0.29667399999999988</v>
+      </c>
+      <c r="D3" s="24">
+        <f>inflow25!J18</f>
+        <v>98.685929999999999</v>
+      </c>
+      <c r="E3" s="23">
+        <f>$D3-$D$2</f>
+        <v>-0.29708999999999719</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4">
+        <v>2.4874000000000001</v>
+      </c>
+      <c r="C4" s="24">
+        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <v>0.32059300000000013</v>
+      </c>
+      <c r="D4" s="32">
+        <v>98.532799999999995</v>
+      </c>
+      <c r="E4" s="23">
+        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <v>-0.45022000000000162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="23">
+        <f>inflow25!I19</f>
+        <v>2.8550430000000002</v>
+      </c>
+      <c r="C7" s="23">
+        <f>B7-B2</f>
+        <v>0.68823600000000029</v>
+      </c>
+      <c r="D7" s="23">
+        <f>inflow25!J19</f>
+        <v>98.016769999999994</v>
+      </c>
+      <c r="E7" s="23">
+        <f>D7-D2</f>
+        <v>-0.96625000000000227</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="23">
+        <f>B2+C9</f>
+        <v>2.7840739999999999</v>
+      </c>
+      <c r="C9" s="23">
+        <f>SUM(C3:C5)</f>
+        <v>0.61726700000000001</v>
+      </c>
+      <c r="D9" s="23">
+        <f>D2+E9</f>
+        <v>98.235709999999997</v>
+      </c>
+      <c r="E9" s="23">
+        <f>SUM(E3:E5)</f>
+        <v>-0.74730999999999881</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B10" s="23">
+        <v>2.8763429999999999</v>
+      </c>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23">
+        <v>97.901719999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added min/max results for FFR 0.25,0.35,0.40 results. Added min/max plotting to 1-iter matlab script
</commit_message>
<xml_diff>
--- a/activeSubspace_results.xlsx
+++ b/activeSubspace_results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="500" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="11"/>
+    <workbookView xWindow="1740" yWindow="500" windowWidth="25360" windowHeight="15820" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="inflow25" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="111">
   <si>
     <t>ER</t>
   </si>
@@ -351,6 +351,18 @@
   </si>
   <si>
     <t>65k iters</t>
+  </si>
+  <si>
+    <t>min MHR</t>
+  </si>
+  <si>
+    <t>max MHR</t>
+  </si>
+  <si>
+    <t>min IHR</t>
+  </si>
+  <si>
+    <t>max IHR</t>
   </si>
 </sst>
 </file>
@@ -432,8 +444,110 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="115">
+  <cellStyleXfs count="149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -831,6 +945,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="168" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -852,11 +969,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="115">
+  <cellStyles count="149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -914,6 +1028,23 @@
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -971,6 +1102,23 @@
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2309,20 +2457,20 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="26"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" ht="19" customHeight="1">
       <c r="A2" s="4"/>
@@ -2351,7 +2499,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19" customHeight="1">
-      <c r="A3" s="27">
+      <c r="A3" s="28">
         <v>0.25</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2373,7 +2521,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" ht="19" customHeight="1">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
@@ -2393,7 +2541,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19" customHeight="1">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
@@ -2413,7 +2561,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="19" customHeight="1">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
@@ -2433,7 +2581,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" ht="19" customHeight="1">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
@@ -2453,7 +2601,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="19" customHeight="1">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
@@ -2473,7 +2621,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="19" customHeight="1">
-      <c r="A9" s="28"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
@@ -2493,7 +2641,7 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="19" customHeight="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2513,7 +2661,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="19" customHeight="1">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="2" t="s">
         <v>20</v>
       </c>
@@ -2533,7 +2681,7 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="19" customHeight="1">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="2" t="s">
         <v>21</v>
       </c>
@@ -2553,7 +2701,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="19" customHeight="1">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
@@ -2573,7 +2721,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" ht="19" customHeight="1">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="2" t="s">
         <v>23</v>
       </c>
@@ -2593,7 +2741,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19" customHeight="1">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="2" t="s">
         <v>24</v>
       </c>
@@ -2613,7 +2761,7 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19" customHeight="1">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="2" t="s">
         <v>25</v>
       </c>
@@ -2633,7 +2781,7 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="19" customHeight="1">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
@@ -2769,7 +2917,7 @@
         <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
         <v>0.37945699999999993</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="25">
         <v>97.968720000000005</v>
       </c>
       <c r="E4" s="23">
@@ -2944,14 +3092,14 @@
         <v>3.2154500000000001</v>
       </c>
       <c r="C4" s="24">
-        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <f t="shared" ref="C4" si="0">$B4-$B$2</f>
         <v>0.54906000000000033</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="25">
         <v>97.129900000000006</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <f t="shared" ref="E4" si="1">$D4-$D$2</f>
         <v>-1.4762999999999948</v>
       </c>
     </row>
@@ -3049,7 +3197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -3118,14 +3266,14 @@
         <v>4.0520500000000004</v>
       </c>
       <c r="C4" s="24">
-        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <f t="shared" ref="C4" si="0">$B4-$B$2</f>
         <v>1.0567600000000006</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="25">
         <v>89.291499999999999</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <f t="shared" ref="E4" si="1">$D4-$D$2</f>
         <v>-8.667199999999994</v>
       </c>
       <c r="F4" t="s">
@@ -3245,31 +3393,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19" customHeight="1">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="29" t="s">
+      <c r="I1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="26"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:14" ht="19" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="7" t="s">
         <v>5</v>
       </c>
@@ -3295,7 +3443,7 @@
       <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:14" ht="19" customHeight="1">
-      <c r="A3" s="30">
+      <c r="A3" s="31">
         <v>0.3</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -3339,7 +3487,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="19" customHeight="1">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="6" t="s">
         <v>13</v>
       </c>
@@ -3371,7 +3519,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="19" customHeight="1">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
@@ -3392,7 +3540,7 @@
       <c r="K5" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="19" customHeight="1">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="6" t="s">
         <v>15</v>
       </c>
@@ -3413,7 +3561,7 @@
       <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:14" ht="19" customHeight="1">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="6" t="s">
         <v>16</v>
       </c>
@@ -3434,7 +3582,7 @@
       <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:14" ht="19" customHeight="1">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="6" t="s">
         <v>17</v>
       </c>
@@ -3455,7 +3603,7 @@
       <c r="K8" s="7"/>
     </row>
     <row r="9" spans="1:14" ht="19" customHeight="1">
-      <c r="A9" s="28"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="6" t="s">
         <v>18</v>
       </c>
@@ -3476,7 +3624,7 @@
       <c r="K9" s="7"/>
     </row>
     <row r="10" spans="1:14" ht="19" customHeight="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
@@ -3497,7 +3645,7 @@
       <c r="K10" s="7"/>
     </row>
     <row r="11" spans="1:14" ht="19" customHeight="1">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="6" t="s">
         <v>20</v>
       </c>
@@ -3518,7 +3666,7 @@
       <c r="K11" s="7"/>
     </row>
     <row r="12" spans="1:14" ht="19" customHeight="1">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="6" t="s">
         <v>21</v>
       </c>
@@ -3539,7 +3687,7 @@
       <c r="K12" s="7"/>
     </row>
     <row r="13" spans="1:14" ht="19" customHeight="1">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
@@ -3560,7 +3708,7 @@
       <c r="K13" s="7"/>
     </row>
     <row r="14" spans="1:14" ht="19" customHeight="1">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="6" t="s">
         <v>23</v>
       </c>
@@ -3581,7 +3729,7 @@
       <c r="K14" s="7"/>
     </row>
     <row r="15" spans="1:14" ht="19" customHeight="1">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="6" t="s">
         <v>24</v>
       </c>
@@ -3602,7 +3750,7 @@
       <c r="K15" s="7"/>
     </row>
     <row r="16" spans="1:14" ht="19" customHeight="1">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="6" t="s">
         <v>25</v>
       </c>
@@ -3623,7 +3771,7 @@
       <c r="K16" s="7"/>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="6" t="s">
         <v>26</v>
       </c>
@@ -4485,31 +4633,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="26"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -4537,7 +4685,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="27">
+      <c r="A3" s="28">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -4562,7 +4710,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4585,7 +4733,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4608,7 +4756,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -4631,7 +4779,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -4654,7 +4802,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4677,7 +4825,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="28"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -4700,7 +4848,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -4721,7 +4869,7 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -4744,7 +4892,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -4767,7 +4915,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -4790,7 +4938,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -4813,7 +4961,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -4836,7 +4984,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -4859,7 +5007,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" ht="19" customHeight="1">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -4980,31 +5128,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="19" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="C1" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
       <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="26"/>
+      <c r="J1" s="27"/>
       <c r="K1" s="4"/>
     </row>
     <row r="2" spans="1:11" ht="19" customHeight="1">
-      <c r="A2" s="26"/>
-      <c r="B2" s="26"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
@@ -5032,7 +5180,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" ht="19" customHeight="1">
-      <c r="A3" s="27">
+      <c r="A3" s="28">
         <v>0.35</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -5057,7 +5205,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="19" customHeight="1">
-      <c r="A4" s="28"/>
+      <c r="A4" s="29"/>
       <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
@@ -5080,7 +5228,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="19" customHeight="1">
-      <c r="A5" s="28"/>
+      <c r="A5" s="29"/>
       <c r="B5" s="3" t="s">
         <v>14</v>
       </c>
@@ -5103,7 +5251,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="19" customHeight="1">
-      <c r="A6" s="28"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -5126,7 +5274,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" ht="19" customHeight="1">
-      <c r="A7" s="28"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
@@ -5149,7 +5297,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="19" customHeight="1">
-      <c r="A8" s="28"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
@@ -5172,7 +5320,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="19" customHeight="1">
-      <c r="A9" s="28"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
@@ -5195,7 +5343,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" ht="19" customHeight="1">
-      <c r="A10" s="28"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
@@ -5218,7 +5366,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="19" customHeight="1">
-      <c r="A11" s="28"/>
+      <c r="A11" s="29"/>
       <c r="B11" s="3" t="s">
         <v>20</v>
       </c>
@@ -5241,7 +5389,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="19" customHeight="1">
-      <c r="A12" s="28"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="3" t="s">
         <v>21</v>
       </c>
@@ -5264,7 +5412,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" ht="19" customHeight="1">
-      <c r="A13" s="28"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="3" t="s">
         <v>22</v>
       </c>
@@ -5287,7 +5435,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" ht="19" customHeight="1">
-      <c r="A14" s="28"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
@@ -5310,7 +5458,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" ht="19" customHeight="1">
-      <c r="A15" s="28"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -5333,7 +5481,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" ht="19" customHeight="1">
-      <c r="A16" s="28"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
@@ -5356,7 +5504,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="19" customHeight="1">
-      <c r="A17" s="28"/>
+      <c r="A17" s="29"/>
       <c r="B17" s="3" t="s">
         <v>26</v>
       </c>
@@ -5431,10 +5579,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -5446,12 +5594,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -5762,39 +5910,87 @@
       <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="14">
+        <v>174881000000</v>
+      </c>
+      <c r="C28" s="14">
+        <v>112561.5</v>
+      </c>
       <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>108</v>
+      </c>
+      <c r="B29" s="14">
+        <v>278825000000</v>
+      </c>
+      <c r="C29" s="14">
+        <v>172764.1</v>
       </c>
       <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="14">
+        <v>176175000000</v>
+      </c>
+      <c r="C30" s="14">
+        <v>114285.6</v>
+      </c>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="14">
+        <v>276149000000</v>
+      </c>
+      <c r="C31" s="14">
+        <v>172284.79999999999</v>
+      </c>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B34" s="14">
         <f>MIN(B$4:B$27)</f>
         <v>195636000000</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C34" s="14">
         <f>MIN(C$4:C$27)</f>
         <v>147609.4</v>
       </c>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B35" s="14">
         <f>MAX(B$4:B$27)</f>
         <v>251214000000</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C35" s="14">
         <f>MAX(C$4:C$27)</f>
         <v>181974.1</v>
       </c>
@@ -5819,7 +6015,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="E28" sqref="E28:E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -5833,18 +6029,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31" t="s">
+      <c r="C1" s="32"/>
+      <c r="D1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="E1" s="32"/>
+      <c r="F1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="31"/>
+      <c r="G1" s="32"/>
     </row>
     <row r="2" spans="1:11" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -6548,10 +6744,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -6563,12 +6759,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -6879,39 +7075,87 @@
       <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="14">
+        <v>183378000000</v>
+      </c>
+      <c r="C28" s="14">
+        <v>142678.39999999999</v>
+      </c>
       <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>108</v>
+      </c>
+      <c r="B29" s="14">
+        <v>296513000000</v>
+      </c>
+      <c r="C29" s="14">
+        <v>218011.9</v>
       </c>
       <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="14">
+        <v>184898000000</v>
+      </c>
+      <c r="C30" s="14">
+        <v>144862.29999999999</v>
+      </c>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="14">
+        <v>294027000000</v>
+      </c>
+      <c r="C31" s="14">
+        <v>217373</v>
+      </c>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B34" s="14">
         <f>MIN(B$4:B$27)</f>
         <v>212363000000</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C34" s="14">
         <f>MIN(C$4:C$27)</f>
         <v>191133.3</v>
       </c>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+      <c r="E34" s="20"/>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B35" s="14">
         <f>MAX(B$4:B$27)</f>
         <v>267270000000</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C35" s="14">
         <f>MAX(C$4:C$27)</f>
         <v>233287.1</v>
       </c>
@@ -6933,10 +7177,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0"/>
@@ -6948,12 +7192,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:9" s="13" customFormat="1" ht="32">
       <c r="A2" s="16" t="s">
@@ -7264,39 +7508,84 @@
       <c r="E27" s="20"/>
     </row>
     <row r="28" spans="1:5">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
+      <c r="A28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B28" s="14">
+        <v>182081000000</v>
+      </c>
+      <c r="C28" s="14">
+        <v>155203.4</v>
+      </c>
       <c r="E28" s="20"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>87</v>
+        <v>108</v>
+      </c>
+      <c r="B29" s="14">
+        <v>291837000000</v>
+      </c>
+      <c r="C29" s="14">
+        <v>237245.4</v>
       </c>
       <c r="E29" s="20"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
+        <v>109</v>
+      </c>
+      <c r="B30" s="14">
+        <v>183801000000</v>
+      </c>
+      <c r="C30" s="14">
+        <v>158178.1</v>
+      </c>
+      <c r="E30" s="20"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>110</v>
+      </c>
+      <c r="B31" s="14">
+        <v>289853000000</v>
+      </c>
+      <c r="C31" s="14">
+        <v>236532.8</v>
+      </c>
+      <c r="E31" s="20"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="E32" s="20"/>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
         <v>85</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B34" s="14">
         <f>MIN(B$4:B$27)</f>
         <v>205002000000</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C34" s="14">
         <f>MIN(C$4:C$27)</f>
         <v>212230.8</v>
       </c>
-      <c r="E30" s="20"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
         <v>86</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B35" s="14">
         <f>MAX(B$4:B$27)</f>
         <v>263216000000</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C35" s="14">
         <f>MAX(C$4:C$27)</f>
         <v>256216.8</v>
       </c>
@@ -7386,14 +7675,14 @@
         <v>2.4874000000000001</v>
       </c>
       <c r="C4" s="24">
-        <f t="shared" ref="C4:C5" si="0">$B4-$B$2</f>
+        <f t="shared" ref="C4" si="0">$B4-$B$2</f>
         <v>0.32059300000000013</v>
       </c>
-      <c r="D4" s="32">
+      <c r="D4" s="25">
         <v>98.532799999999995</v>
       </c>
       <c r="E4" s="23">
-        <f t="shared" ref="E4:E5" si="1">$D4-$D$2</f>
+        <f t="shared" ref="E4" si="1">$D4-$D$2</f>
         <v>-0.45022000000000162</v>
       </c>
     </row>

</xml_diff>